<commit_message>
Jupiter notebook initial commit and feature engineering
</commit_message>
<xml_diff>
--- a/data/processed/Cleaned_Japan_Life_Expectancy.xlsx
+++ b/data/processed/Cleaned_Japan_Life_Expectancy.xlsx
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2496333374177621</v>
+        <v>84.65000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2901618929016188</v>
+        <v>224.4</v>
       </c>
       <c r="D2" t="n">
         <v>13.6</v>
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1.47813712464157</v>
+        <v>83.79000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4034869240348691</v>
+        <v>242.6</v>
       </c>
       <c r="D3" t="n">
         <v>11.3</v>
@@ -714,10 +714,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3.46708219143082</v>
+        <v>82.8</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2160647571606475</v>
+        <v>212.5</v>
       </c>
       <c r="D4" t="n">
         <v>11.4</v>
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.09190268415210942</v>
+        <v>84.48</v>
       </c>
       <c r="C5" t="n">
-        <v>0.174346201743462</v>
+        <v>205.8</v>
       </c>
       <c r="D5" t="n">
         <v>14.7</v>
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.5740711851919414</v>
+        <v>84.23999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6158156911581567</v>
+        <v>276.7</v>
       </c>
       <c r="D6" t="n">
         <v>14.2</v>
@@ -942,10 +942,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7719825468775421</v>
+        <v>84.91</v>
       </c>
       <c r="C7" t="n">
-        <v>0.4987546699875465</v>
+        <v>257.9</v>
       </c>
       <c r="D7" t="n">
         <v>12.9</v>
@@ -1018,10 +1018,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0286394411078486</v>
+        <v>84.54000000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8225404732254047</v>
+        <v>309.9</v>
       </c>
       <c r="D8" t="n">
         <v>14.2</v>
@@ -1094,10 +1094,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1.638859958321533</v>
+        <v>83.70999999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1737235367372352</v>
+        <v>205.7</v>
       </c>
       <c r="D9" t="n">
         <v>11.6</v>
@@ -1170,10 +1170,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3701754626776916</v>
+        <v>84.70999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2907845579078454</v>
+        <v>224.5</v>
       </c>
       <c r="D10" t="n">
         <v>13.4</v>
@@ -1246,10 +1246,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.734794018871876</v>
+        <v>84.16</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3486924034869241</v>
+        <v>233.8</v>
       </c>
       <c r="D11" t="n">
         <v>14.7</v>
@@ -1322,10 +1322,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.073337860027437</v>
+        <v>85.06</v>
       </c>
       <c r="C12" t="n">
-        <v>0.5560398505603985</v>
+        <v>267.1</v>
       </c>
       <c r="D12" t="n">
         <v>16.1</v>
@@ -1398,10 +1398,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-1.056239686231745</v>
+        <v>84</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4576587795765878</v>
+        <v>251.3</v>
       </c>
       <c r="D13" t="n">
         <v>14.1</v>
@@ -1474,10 +1474,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5710790047776311</v>
+        <v>84.81</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5498132004981322</v>
+        <v>266.1</v>
       </c>
       <c r="D14" t="n">
         <v>13.7</v>
@@ -1550,10 +1550,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-1.21696251991168</v>
+        <v>83.92</v>
       </c>
       <c r="C15" t="n">
-        <v>0.09962640099626396</v>
+        <v>193.8</v>
       </c>
       <c r="D15" t="n">
         <v>12.7</v>
@@ -1626,10 +1626,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1.073337860027437</v>
+        <v>85.06</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7085927770859279</v>
+        <v>291.6</v>
       </c>
       <c r="D16" t="n">
         <v>14.7</v>
@@ -1702,10 +1702,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-1.35759499938164</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1836861768368616</v>
+        <v>207.3</v>
       </c>
       <c r="D17" t="n">
         <v>12.7</v>
@@ -1778,10 +1778,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.1491815663677781</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6986301369863013</v>
+        <v>290</v>
       </c>
       <c r="D18" t="n">
         <v>14.3</v>
@@ -1854,10 +1854,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.5740711851919414</v>
+        <v>84.23999999999999</v>
       </c>
       <c r="C19" t="n">
-        <v>0.658779576587796</v>
+        <v>283.6</v>
       </c>
       <c r="D19" t="n">
         <v>14.4</v>
@@ -1930,10 +1930,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.8925246721375001</v>
+        <v>84.97</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2814445828144456</v>
+        <v>223</v>
       </c>
       <c r="D20" t="n">
         <v>15.1</v>
@@ -2006,10 +2006,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-0.413348351512007</v>
+        <v>84.31999999999999</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8978829389788294</v>
+        <v>322</v>
       </c>
       <c r="D21" t="n">
         <v>12.9</v>
@@ -2082,10 +2082,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.093428214237411</v>
+        <v>85.06999999999999</v>
       </c>
       <c r="C22" t="n">
-        <v>0.742216687422167</v>
+        <v>297</v>
       </c>
       <c r="D22" t="n">
         <v>12.8</v>
@@ -2158,10 +2158,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1.455054590017285</v>
+        <v>85.25</v>
       </c>
       <c r="C23" t="n">
-        <v>0.9638854296388546</v>
+        <v>332.6</v>
       </c>
       <c r="D23" t="n">
         <v>13.3</v>
@@ -2234,10 +2234,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.2295429832077596</v>
+        <v>84.64</v>
       </c>
       <c r="C24" t="n">
-        <v>0.3349937733499375</v>
+        <v>231.6</v>
       </c>
       <c r="D24" t="n">
         <v>12.2</v>
@@ -2310,10 +2310,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1692719205777806</v>
+        <v>84.61</v>
       </c>
       <c r="C25" t="n">
-        <v>0.4265255292652552</v>
+        <v>246.3</v>
       </c>
       <c r="D25" t="n">
         <v>12.2</v>
@@ -2386,10 +2386,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.2928062262520489</v>
+        <v>84.38</v>
       </c>
       <c r="C26" t="n">
-        <v>0.483810709838107</v>
+        <v>255.5</v>
       </c>
       <c r="D26" t="n">
         <v>12.2</v>
@@ -2462,10 +2462,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.87695202842711</v>
+        <v>85.45999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>0.4109589041095891</v>
+        <v>243.8</v>
       </c>
       <c r="D27" t="n">
         <v>16.9</v>
@@ -2538,10 +2538,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.6343422478219205</v>
+        <v>84.20999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8798256537982567</v>
+        <v>319.1</v>
       </c>
       <c r="D28" t="n">
         <v>12.3</v>
@@ -2614,10 +2614,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1.314422110547353</v>
+        <v>85.18000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6183063511830635</v>
+        <v>277.1</v>
       </c>
       <c r="D29" t="n">
         <v>15.2</v>
@@ -2690,10 +2690,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.1923544552020649</v>
+        <v>84.43000000000001</v>
       </c>
       <c r="C30" t="n">
-        <v>0.1650062266500623</v>
+        <v>204.3</v>
       </c>
       <c r="D30" t="n">
         <v>13.6</v>
@@ -2766,10 +2766,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.7719825468775421</v>
+        <v>84.91</v>
       </c>
       <c r="C31" t="n">
-        <v>0.6805728518057286</v>
+        <v>287.1</v>
       </c>
       <c r="D31" t="n">
         <v>13.5</v>
@@ -2842,10 +2842,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1.15369927686739</v>
+        <v>85.09999999999999</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8860523038605232</v>
+        <v>320.1</v>
       </c>
       <c r="D32" t="n">
         <v>13.9</v>
@@ -2918,10 +2918,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.433438705721981</v>
+        <v>84.31</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4943960149439601</v>
+        <v>257.2</v>
       </c>
       <c r="D33" t="n">
         <v>13.9</v>
@@ -2994,10 +2994,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.875426498341808</v>
+        <v>84.09</v>
       </c>
       <c r="C34" t="n">
-        <v>0.6718555417185554</v>
+        <v>285.7</v>
       </c>
       <c r="D34" t="n">
         <v>13.2</v>
@@ -3070,10 +3070,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.1491815663677781</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7004981320049815</v>
+        <v>290.3</v>
       </c>
       <c r="D35" t="n">
         <v>13.1</v>
@@ -3146,10 +3146,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.2928062262520489</v>
+        <v>84.38</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>177.8</v>
       </c>
       <c r="D36" t="n">
         <v>15.1</v>
@@ -3222,10 +3222,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1.957313445267091</v>
+        <v>85.5</v>
       </c>
       <c r="C37" t="n">
-        <v>0.3642590286425902</v>
+        <v>236.3</v>
       </c>
       <c r="D37" t="n">
         <v>14.9</v>
@@ -3298,10 +3298,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.7920729010875446</v>
+        <v>84.92</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7428393524283936</v>
+        <v>297.1</v>
       </c>
       <c r="D38" t="n">
         <v>12.9</v>
@@ -3374,10 +3374,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.0286394411078486</v>
+        <v>84.54000000000001</v>
       </c>
       <c r="C39" t="n">
-        <v>0.2590286425902864</v>
+        <v>219.4</v>
       </c>
       <c r="D39" t="n">
         <v>13.9</v>
@@ -3450,10 +3450,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-1.1566914572817</v>
+        <v>83.95</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3679950186799501</v>
+        <v>236.9</v>
       </c>
       <c r="D40" t="n">
         <v>13.2</v>
@@ -3526,10 +3526,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.353077288882028</v>
+        <v>84.34999999999999</v>
       </c>
       <c r="C41" t="n">
-        <v>1</v>
+        <v>338.4</v>
       </c>
       <c r="D41" t="n">
         <v>13.1</v>
@@ -3602,10 +3602,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.5911693589876051</v>
+        <v>84.81999999999999</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8910336239103362</v>
+        <v>320.9</v>
       </c>
       <c r="D42" t="n">
         <v>12.8</v>
@@ -3678,10 +3678,10 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.2094526289977571</v>
+        <v>84.63</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8530510585305107</v>
+        <v>314.8</v>
       </c>
       <c r="D43" t="n">
         <v>13.4</v>
@@ -3754,10 +3754,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.6715307758275866</v>
+        <v>84.86</v>
       </c>
       <c r="C44" t="n">
-        <v>0.521170610211706</v>
+        <v>261.5</v>
       </c>
       <c r="D44" t="n">
         <v>15.7</v>
@@ -3830,10 +3830,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.6544326020318945</v>
+        <v>84.2</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8094645080946452</v>
+        <v>307.8</v>
       </c>
       <c r="D45" t="n">
         <v>12.9</v>
@@ -3906,10 +3906,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.2727158720420464</v>
+        <v>84.39</v>
       </c>
       <c r="C46" t="n">
-        <v>0.3200498132004981</v>
+        <v>229.2</v>
       </c>
       <c r="D46" t="n">
         <v>12.2</v>
@@ -3982,10 +3982,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.49370976835196</v>
+        <v>84.28</v>
       </c>
       <c r="C47" t="n">
-        <v>0.5124533001245331</v>
+        <v>260.1</v>
       </c>
       <c r="D47" t="n">
         <v>13.5</v>
@@ -4058,10 +4058,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.6112597131976076</v>
+        <v>84.83</v>
       </c>
       <c r="C48" t="n">
-        <v>0.4501867995018678</v>
+        <v>250.1</v>
       </c>
       <c r="D48" t="n">
         <v>15.9</v>

</xml_diff>